<commit_message>
Inclusão de validação para remoção de filial quando houver aluno ou colaborador associado.
</commit_message>
<xml_diff>
--- a/Casos de teste.xlsx
+++ b/Casos de teste.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="308">
   <si>
     <t>Descrição</t>
   </si>
@@ -3624,6 +3624,21 @@
   </si>
   <si>
     <t>Verificar se é possível agendar avaliação física em dia da semana e horário não aprovisionados e anteriores à data atual.</t>
+  </si>
+  <si>
+    <t>RFN1.2</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Evitar remoção de filial.</t>
+  </si>
+  <si>
+    <t>Apresentação de mensagem de erro indicando “Existem alunos e colaboradores associados à filial.”.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remover uma filial que contenha alunos ou colaboradores associados. </t>
   </si>
 </sst>
 </file>
@@ -4267,10 +4282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,50 +4413,50 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B7" s="15">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>236</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>3</v>
@@ -4458,19 +4473,19 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>3</v>
@@ -4487,77 +4502,77 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B10" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="F10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="15">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="15">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>239</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>3</v>
@@ -4574,77 +4589,77 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B13" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="F13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B14" s="15">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>3</v>
@@ -4661,19 +4676,19 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>278</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>135</v>
+        <v>279</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>129</v>
+        <v>296</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>3</v>
@@ -4690,19 +4705,19 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>282</v>
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>3</v>
@@ -4719,48 +4734,48 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B18" s="15">
         <v>5</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>3</v>
@@ -4777,106 +4792,106 @@
     </row>
     <row r="19" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B20" s="15">
         <v>6</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="F20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B21" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="F21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B22" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C22" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D22" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E22" s="25" t="s">
         <v>133</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>3</v>
@@ -4893,19 +4908,19 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>137</v>
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>3</v>
@@ -4922,19 +4937,19 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="15">
-        <v>7</v>
+        <v>67</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>248</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>151</v>
+        <v>23</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>218</v>
+        <v>137</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>3</v>
@@ -4951,19 +4966,19 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>249</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="15">
+        <v>7</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>139</v>
+        <v>151</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="F25" s="13" t="s">
         <v>3</v>
@@ -4980,19 +4995,19 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>141</v>
+        <v>68</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="F26" s="13" t="s">
         <v>3</v>
@@ -5009,19 +5024,19 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="15">
-        <v>8</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>285</v>
+        <v>141</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>3</v>
@@ -5038,77 +5053,77 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="15">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B29" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
+      <c r="F29" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="15">
+      <c r="B30" s="15">
         <v>9</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>3</v>
@@ -5125,135 +5140,135 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B32" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="F32" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B33" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="F33" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B34" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F33" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
+      <c r="F34" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B35" s="18">
         <v>10</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H34" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>256</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="F35" s="13" t="s">
         <v>3</v>
@@ -5270,19 +5285,19 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>169</v>
+        <v>37</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>3</v>
@@ -5299,19 +5314,19 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>171</v>
+        <v>38</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="F37" s="13" t="s">
         <v>3</v>
@@ -5328,19 +5343,19 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="18">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>258</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>172</v>
+        <v>40</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>232</v>
+        <v>171</v>
       </c>
       <c r="F38" s="13" t="s">
         <v>3</v>
@@ -5357,48 +5372,48 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="18">
+        <v>11</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B40" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>3</v>
@@ -5415,109 +5430,109 @@
     </row>
     <row r="41" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B42" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F41" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
+      <c r="F42" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B43" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="F42" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
+      <c r="F43" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B44" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="18">
-        <v>12</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>4</v>
-      </c>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
       <c r="H44" s="28">
         <v>43738</v>
       </c>
@@ -5527,193 +5542,193 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="18">
+        <v>12</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B46" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F45" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H45" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
+      <c r="F46" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B47" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="F46" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H46" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="17" t="s">
+      <c r="F47" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B48" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F47" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H47" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
+      <c r="F48" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="18">
+      <c r="B49" s="18">
         <v>13</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F48" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H48" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I48" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
+      <c r="F49" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H49" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B50" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F49" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H49" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I49" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="17" t="s">
+      <c r="F50" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="18">
+      <c r="B51" s="18">
         <v>14</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D50" s="27" t="s">
+      <c r="D51" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="F50" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="F51" s="13" t="s">
         <v>3</v>
@@ -5730,19 +5745,19 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>3</v>
@@ -5759,48 +5774,48 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H53" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="18">
+      <c r="B54" s="18">
         <v>15</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H53" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I53" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>3</v>
@@ -5817,48 +5832,48 @@
     </row>
     <row r="55" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H55" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="18">
+      <c r="B56" s="18">
         <v>16</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G55" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H55" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I55" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="F56" s="13" t="s">
         <v>3</v>
@@ -5875,19 +5890,19 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>196</v>
+        <v>96</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>3</v>
@@ -5904,77 +5919,77 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H58" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B59" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F58" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H58" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="17" t="s">
+      <c r="F59" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B60" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D60" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="F59" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G59" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H59" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I59" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>203</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="F60" s="13" t="s">
         <v>3</v>
@@ -5991,106 +6006,106 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B62" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D61" s="27" t="s">
+      <c r="D62" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F61" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H61" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I61" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="17" t="s">
+      <c r="F62" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B62" s="18">
+      <c r="B63" s="18">
         <v>17</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="F62" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H62" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I62" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="17" t="s">
+      <c r="F63" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="18" t="s">
+      <c r="B64" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>206</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G63" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H63" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I63" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" s="18">
-        <v>18</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="F64" s="13" t="s">
         <v>3</v>
@@ -6107,16 +6122,16 @@
     </row>
     <row r="65" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B65" s="18">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>230</v>
@@ -6134,18 +6149,18 @@
         <v>294</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B66" s="18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>230</v>
@@ -6163,21 +6178,21 @@
         <v>294</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B67" s="18">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F67" s="13" t="s">
         <v>3</v>
@@ -6194,30 +6209,59 @@
     </row>
     <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B68" s="18">
+        <v>21</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="B68" s="18">
+      <c r="B69" s="18">
         <v>22</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F68" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H68" s="28">
-        <v>43738</v>
-      </c>
-      <c r="I68" s="13" t="s">
+      <c r="F69" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H69" s="28">
+        <v>43738</v>
+      </c>
+      <c r="I69" s="13" t="s">
         <v>294</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Inclusão de bloqueio e validação para agendamento de aula experimental e avaliação física no dia atual.
</commit_message>
<xml_diff>
--- a/Casos de teste.xlsx
+++ b/Casos de teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrunaCarolineTegon\Downloads\FACULDADE\TEST RESULTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A073EB8-9574-4BBD-83C0-E092AE4F5EB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAAFDFB-4A50-4CD5-8702-CB210A63D80B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2469,18 +2469,6 @@
     <t xml:space="preserve">Não há limite de agendamentos de aula experimental para o dia da semana e horário disponibilizados pelo administrador ou colaborador, a quantidade de agendamentos dependerá das aprovações de administradores e colaboradores das filiais. </t>
   </si>
   <si>
-    <t>Verificar se é possível agendar aula experimental em dia da semana e horário não aprovisionados e anteriores a data atual.</t>
-  </si>
-  <si>
-    <t>Bloqueio de data do agendamento e horário ao agendamento de avaliação física em dias da semana e horários não fornecidos por administrador ou colaboradores e anteriores à data atual.</t>
-  </si>
-  <si>
-    <t>Bloqueio de data do agendamento e horário ao agendamento de aula experimental em dias da semana e horários não fornecidos por administrador ou colaboradores e anteriores à data atual.</t>
-  </si>
-  <si>
-    <t>Verificar se é possível agendar avaliação física em dia da semana e horário não aprovisionados e anteriores à data atual.</t>
-  </si>
-  <si>
     <t>RFN1.2</t>
   </si>
   <si>
@@ -3684,6 +3672,18 @@
       </rPr>
       <t xml:space="preserve"> dos dados no sistema. </t>
     </r>
+  </si>
+  <si>
+    <t>Verificar se é possível agendar avaliação física em dia da semana e horário não aprovisionados, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Verificar se é possível agendar aula experimental em dia da semana e horário não aprovisionados, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Bloqueio de data do agendamento e horário ao agendamento de avaliação física em dias da semana e horários não fornecidos por administrador ou colaboradores, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Bloqueio de data do agendamento e horário ao agendamento de aula experimental em dias da semana e horários não fornecidos por administrador ou colaboradores, anteriores à data atual ou na data atual.</t>
   </si>
 </sst>
 </file>
@@ -3978,24 +3978,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4058,6 +4040,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4376,7 +4376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F54" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -4393,30 +4393,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -4447,1888 +4447,1888 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="F4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="8">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="8">
+        <v>6</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8">
+        <v>7</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="8">
+        <v>8</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="21">
+        <v>9</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="B31" s="24">
+        <v>9.1</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="B32" s="26">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="14">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="17">
+        <v>9.4</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="19">
+        <v>10</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="19">
+        <v>11</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="19">
+        <v>12</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="19">
+        <v>13</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="19">
+        <v>14</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" s="19">
+        <v>15</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="19">
+        <v>16</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B56" s="19">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" s="19">
+        <v>16.2</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="B58" s="19">
+        <v>16.3</v>
+      </c>
+      <c r="C58" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="14">
-        <v>2</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="D58" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B59" s="19">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E59" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14">
-        <v>3</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="14">
-        <v>4</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="11" t="s">
+      <c r="F59" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B60" s="19">
+        <v>16.5</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" s="19">
         <v>17</v>
       </c>
-      <c r="B18" s="14">
-        <v>5</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="C61" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I62" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="B63" s="19">
         <v>18</v>
       </c>
-      <c r="D18" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="11" t="s">
+      <c r="C63" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I63" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B64" s="19">
         <v>19</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="11" t="s">
+      <c r="C64" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="10" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B65" s="19">
         <v>20</v>
       </c>
-      <c r="B20" s="14">
-        <v>6</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="C65" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="19">
         <v>21</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>274</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="13" t="s">
+      <c r="C66" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B67" s="19">
         <v>22</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="C24" s="13" t="s">
+      <c r="C67" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="B68" s="19">
         <v>23</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="14">
-        <v>7</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="14">
-        <v>8</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="27">
-        <v>9</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="B31" s="30">
-        <v>9.1</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>277</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G31" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="25" t="s">
-        <v>280</v>
-      </c>
-      <c r="B32" s="32">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="20">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="B34" s="23">
-        <v>9.4</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="25">
-        <v>10</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="C36" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>285</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="C38" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="25">
-        <v>11</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G39" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I39" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H40" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="16" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>208</v>
-      </c>
-      <c r="C41" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="C42" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="D42" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="C43" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I43" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="16" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="C44" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="25">
-        <v>12</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I45" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="16" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="C46" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>212</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>238</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="F47" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I47" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="25">
-        <v>13</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I49" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B50" s="25">
-        <v>14</v>
-      </c>
-      <c r="C50" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D50" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E50" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I50" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>214</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="E51" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I51" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="E52" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G52" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" s="25">
-        <v>15</v>
-      </c>
-      <c r="C53" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G54" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I54" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="25">
-        <v>16</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I55" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="B56" s="25">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>253</v>
-      </c>
-      <c r="D56" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B57" s="25">
-        <v>16.2</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="F57" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H57" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I57" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="16" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B58" s="25">
-        <v>16.3</v>
-      </c>
-      <c r="C58" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="D58" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G58" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I58" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B59" s="25">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="C59" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E59" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F59" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G59" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I59" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="22" t="s">
-        <v>269</v>
-      </c>
-      <c r="B60" s="25">
-        <v>16.5</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="E60" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F60" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G60" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I60" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" s="25">
-        <v>17</v>
-      </c>
-      <c r="C61" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="E61" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="F61" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G61" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I61" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>217</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E62" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H62" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I62" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="B63" s="25">
-        <v>18</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="E63" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="F63" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G63" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H63" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I63" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="16" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" s="25">
-        <v>19</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="13" t="s">
+      <c r="C68" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="F64" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G64" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H64" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I64" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="16" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" s="25">
-        <v>20</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E65" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H65" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I65" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" s="16" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" s="25">
-        <v>21</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E66" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F66" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H66" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I66" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B67" s="25">
-        <v>22</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="E67" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F67" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H67" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I67" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="B68" s="25">
-        <v>23</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E68" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="F68" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H68" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="I68" s="14" t="s">
+      <c r="F68" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="I68" s="8" t="s">
         <v>233</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Notificação por email somente com inclusão de comentário no ticket efetuado pelo analista e atualização das datas de re-teste.
</commit_message>
<xml_diff>
--- a/Casos de teste.xlsx
+++ b/Casos de teste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrunaCarolineTegon\Downloads\FACULDADE\TEST RESULTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrunaCarolineTegon\Downloads\FACULDADE\TEST RESULTS\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAAFDFB-4A50-4CD5-8702-CB210A63D80B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6190C59-BAE3-491D-808F-D6CD04810AC0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="293">
   <si>
     <t>Descrição</t>
   </si>
@@ -956,12 +956,6 @@
     </r>
   </si>
   <si>
-    <t>Apresentação de mensagem de erro indicando “Manual já cadastrado.” ao registro ou edição de manual para analistas.</t>
-  </si>
-  <si>
-    <t>Apresentação de mensagem de erro indicando “Arquivo já cadastrado.” ao registro ou edição de manual para analistas.</t>
-  </si>
-  <si>
     <t>Apresentação de relatórios ao nível de acesso de administrador.</t>
   </si>
   <si>
@@ -2783,9 +2777,6 @@
     <t>Verificar se as avaliações físicas são apresentadas em conformidade ao nível de acesso.</t>
   </si>
   <si>
-    <t>20/10/2019</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Interface para </t>
     </r>
@@ -2835,7 +2826,34 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Verificar se notificações são enviadas ao usuário após registro de </t>
+      <t xml:space="preserve">Edição de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>tickets.</t>
+    </r>
+  </si>
+  <si>
+    <t>RFN16.1</t>
+  </si>
+  <si>
+    <t>RFN16.3</t>
+  </si>
+  <si>
+    <t>RFN16.4</t>
+  </si>
+  <si>
+    <t>RFN16.5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bloqueio de edição de título e descrição do </t>
     </r>
     <r>
       <rPr>
@@ -2854,7 +2872,41 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">, comentários de analistas ao </t>
+      <t xml:space="preserve"> após a criação, possibilitando somente a modificação de classificação, prioridade e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> realizada por analistas</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verificar se existe possibilidade de edição de título e descrição de </t>
     </r>
     <r>
       <rPr>
@@ -2873,26 +2925,641 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> e atualização de </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> do </t>
+      <t xml:space="preserve"> após criação; verificar se existe possibilidade de modificação de classificação, prioridade e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">status </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>por analistas</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Acesso aos </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>tickets.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Evitar duplicidade de CPF e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> do colaborador.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Apresentação de mensagem de erro indicando “CPF já cadastrado.” e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> já cadastrado.” ao registro ou edição de colaborador.</t>
+    </r>
+  </si>
+  <si>
+    <t>RFI9.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> inválido.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Apresentação de mensagens de erro indicando “</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> inválido.”.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Preencher o campo </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> com </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> não cadastrado na base de dados. </t>
+    </r>
+  </si>
+  <si>
+    <t>RFI9.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> inválido.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Apresentação de mensagens de erro indicando “</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> inválido.”.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modificar o </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> fornecido para redefinição de senha, reutilizá-lo ou utilizá-lo após vinte e quatro horas.</t>
+    </r>
+  </si>
+  <si>
+    <t>A criação de eventos é limitada à filial em que o administrador ou colaborador está cadastrado.</t>
+  </si>
+  <si>
+    <t>Verificar se a criação de eventos é limitada à filial em que o administrador ou colaborador está cadastrado.</t>
+  </si>
+  <si>
+    <t>Preencher campo horário em formato hora-minuto (hh:mm).</t>
+  </si>
+  <si>
+    <t>Campo livre para digitação de horário no formato hora-minuto com dois digitos (hh:mm) baseado em sistema vinte e quatro horas ao cadastro de eventos.</t>
+  </si>
+  <si>
+    <t>Acessar menu lateral e clicar na opção agendamento. Preencher as informações requisitadas e clicar em salvar.</t>
+  </si>
+  <si>
+    <t>RFN18</t>
+  </si>
+  <si>
+    <t>RFI23</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Backup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>restore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Operações de </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>backup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> de dados dos módulos do sistema e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>restore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> realizadas com sucesso. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Efetuar </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, acessar o menu suporte e clicar na opção </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>backup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>restore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Executar o </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>backup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> e, em seguida, realizar o </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>restore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> dos dados no sistema. </t>
+    </r>
+  </si>
+  <si>
+    <t>Verificar se é possível agendar avaliação física em dia da semana e horário não aprovisionados, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Verificar se é possível agendar aula experimental em dia da semana e horário não aprovisionados, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Bloqueio de data do agendamento e horário ao agendamento de avaliação física em dias da semana e horários não fornecidos por administrador ou colaboradores, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Bloqueio de data do agendamento e horário ao agendamento de aula experimental em dias da semana e horários não fornecidos por administrador ou colaboradores, anteriores à data atual ou na data atual.</t>
+  </si>
+  <si>
+    <t>Apresentação de mensagem de erro indicando “Manual já cadastrado.” ao registro manual para analistas.</t>
+  </si>
+  <si>
+    <t>Apresentação de mensagem de erro indicando “Arquivo já cadastrado.” ao registro de manual para analistas.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Envio de notificações ao </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> do usuário informando sobre comentários do analista no </t>
     </r>
     <r>
       <rPr>
@@ -2907,34 +3574,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Edição de </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>tickets.</t>
-    </r>
-  </si>
-  <si>
-    <t>RFN16.1</t>
-  </si>
-  <si>
-    <t>RFN16.3</t>
-  </si>
-  <si>
-    <t>RFN16.4</t>
-  </si>
-  <si>
-    <t>RFN16.5</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Bloqueio de edição de título e descrição do </t>
+      <t xml:space="preserve">Verificar se notificações são enviadas ao usuário após comentários de analistas ao </t>
     </r>
     <r>
       <rPr>
@@ -2953,737 +3593,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> após a criação, possibilitando somente a modificação de classificação, prioridade e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> realizada por analistas</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Verificar se existe possibilidade de edição de título e descrição de </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ticket</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> após criação; verificar se existe possibilidade de modificação de classificação, prioridade e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">status </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>por analistas</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Acesso aos </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>tickets.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Envio de notificações ao </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> do usuário informando sobre o registro do </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ticket</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (aguardando verificação), comentários do analista e atualização de </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>status</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> do </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ticket.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Evitar duplicidade de CPF e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> do colaborador.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Apresentação de mensagem de erro indicando “CPF já cadastrado.” e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> já cadastrado.” ao registro ou edição de colaborador.</t>
-    </r>
-  </si>
-  <si>
-    <t>RFI9.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> inválido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Apresentação de mensagens de erro indicando “</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>E</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> inválido.”.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Preencher o campo </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> com </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>e</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>mail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> não cadastrado na base de dados. </t>
-    </r>
-  </si>
-  <si>
-    <t>RFI9.2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> inválido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Apresentação de mensagens de erro indicando “</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> inválido.”.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Modificar o </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>link</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> fornecido para redefinição de senha, reutilizá-lo ou utilizá-lo após vinte e quatro horas.</t>
-    </r>
-  </si>
-  <si>
-    <t>A criação de eventos é limitada à filial em que o administrador ou colaborador está cadastrado.</t>
-  </si>
-  <si>
-    <t>Verificar se a criação de eventos é limitada à filial em que o administrador ou colaborador está cadastrado.</t>
-  </si>
-  <si>
-    <t>Preencher campo horário em formato hora-minuto (hh:mm).</t>
-  </si>
-  <si>
-    <t>Campo livre para digitação de horário no formato hora-minuto com dois digitos (hh:mm) baseado em sistema vinte e quatro horas ao cadastro de eventos.</t>
-  </si>
-  <si>
-    <t>Acessar menu lateral e clicar na opção agendamento. Preencher as informações requisitadas e clicar em salvar.</t>
-  </si>
-  <si>
-    <t>RFN18</t>
-  </si>
-  <si>
-    <t>RFI23</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Backup</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>restore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Operações de </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>backup</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> de dados dos módulos do sistema e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>restore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> realizadas com sucesso. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Efetuar </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>login</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, acessar o menu suporte e clicar na opção </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>backup</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> e </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>restore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. Executar o </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>backup</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> e, em seguida, realizar o </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>restore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> dos dados no sistema. </t>
-    </r>
-  </si>
-  <si>
-    <t>Verificar se é possível agendar avaliação física em dia da semana e horário não aprovisionados, anteriores à data atual ou na data atual.</t>
-  </si>
-  <si>
-    <t>Verificar se é possível agendar aula experimental em dia da semana e horário não aprovisionados, anteriores à data atual ou na data atual.</t>
-  </si>
-  <si>
-    <t>Bloqueio de data do agendamento e horário ao agendamento de avaliação física em dias da semana e horários não fornecidos por administrador ou colaboradores, anteriores à data atual ou na data atual.</t>
-  </si>
-  <si>
-    <t>Bloqueio de data do agendamento e horário ao agendamento de aula experimental em dias da semana e horários não fornecidos por administrador ou colaboradores, anteriores à data atual ou na data atual.</t>
   </si>
 </sst>
 </file>
@@ -4376,8 +4287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F54" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4407,7 +4318,7 @@
     </row>
     <row r="2" spans="1:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="30" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -4420,10 +4331,10 @@
     </row>
     <row r="3" spans="1:9" ht="40" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -4435,7 +4346,7 @@
         <v>48</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>47</v>
@@ -4461,7 +4372,7 @@
         <v>125</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>3</v>
@@ -4469,11 +4380,11 @@
       <c r="G4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>257</v>
+      <c r="H4" s="9">
+        <v>43749</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4481,10 +4392,10 @@
         <v>52</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>105</v>
@@ -4498,28 +4409,28 @@
       <c r="G5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>257</v>
+      <c r="H5" s="9">
+        <v>43749</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>239</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>3</v>
@@ -4527,11 +4438,11 @@
       <c r="G6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>257</v>
+      <c r="H6" s="9">
+        <v>43749</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -4548,7 +4459,7 @@
         <v>126</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>3</v>
@@ -4556,11 +4467,11 @@
       <c r="G7" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>257</v>
+      <c r="H7" s="9">
+        <v>43749</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4568,7 +4479,7 @@
         <v>53</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>7</v>
@@ -4585,11 +4496,11 @@
       <c r="G8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>257</v>
+      <c r="H8" s="9">
+        <v>43749</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4597,13 +4508,13 @@
         <v>54</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>107</v>
@@ -4614,11 +4525,11 @@
       <c r="G9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>257</v>
+      <c r="H9" s="9">
+        <v>43749</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4626,7 +4537,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>55</v>
@@ -4643,11 +4554,11 @@
       <c r="G10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>257</v>
+      <c r="H10" s="9">
+        <v>43749</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -4664,7 +4575,7 @@
         <v>127</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>3</v>
@@ -4672,11 +4583,11 @@
       <c r="G11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>257</v>
+      <c r="H11" s="9">
+        <v>43749</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4684,7 +4595,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>13</v>
@@ -4701,11 +4612,11 @@
       <c r="G12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>257</v>
+      <c r="H12" s="9">
+        <v>43749</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4713,16 +4624,16 @@
         <v>56</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>3</v>
@@ -4730,11 +4641,11 @@
       <c r="G13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>257</v>
+      <c r="H13" s="9">
+        <v>43749</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -4751,7 +4662,7 @@
         <v>128</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>3</v>
@@ -4759,11 +4670,11 @@
       <c r="G14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>257</v>
+      <c r="H14" s="9">
+        <v>43749</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4771,16 +4682,16 @@
         <v>58</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>3</v>
@@ -4788,11 +4699,11 @@
       <c r="G15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>257</v>
+      <c r="H15" s="9">
+        <v>43749</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4800,7 +4711,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>16</v>
@@ -4817,11 +4728,11 @@
       <c r="G16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>257</v>
+      <c r="H16" s="9">
+        <v>43749</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4829,28 +4740,28 @@
         <v>60</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>223</v>
-      </c>
       <c r="F17" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="9" t="s">
-        <v>257</v>
+      <c r="H17" s="9">
+        <v>43749</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4867,7 +4778,7 @@
         <v>129</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>3</v>
@@ -4875,11 +4786,11 @@
       <c r="G18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>257</v>
+      <c r="H18" s="9">
+        <v>43749</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -4887,13 +4798,13 @@
         <v>19</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>113</v>
@@ -4904,11 +4815,11 @@
       <c r="G19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>257</v>
+      <c r="H19" s="9">
+        <v>43749</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -4925,7 +4836,7 @@
         <v>130</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>3</v>
@@ -4933,11 +4844,11 @@
       <c r="G20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>257</v>
+      <c r="H20" s="9">
+        <v>43749</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4945,16 +4856,16 @@
         <v>62</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>3</v>
@@ -4962,11 +4873,11 @@
       <c r="G21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="9" t="s">
-        <v>257</v>
+      <c r="H21" s="9">
+        <v>43749</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4974,7 +4885,7 @@
         <v>63</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>22</v>
@@ -4991,11 +4902,11 @@
       <c r="G22" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H22" s="9" t="s">
-        <v>257</v>
+      <c r="H22" s="9">
+        <v>43749</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5003,7 +4914,7 @@
         <v>64</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>16</v>
@@ -5020,11 +4931,11 @@
       <c r="G23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="9" t="s">
-        <v>257</v>
+      <c r="H23" s="9">
+        <v>43749</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5032,7 +4943,7 @@
         <v>65</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>23</v>
@@ -5049,11 +4960,11 @@
       <c r="G24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="9" t="s">
-        <v>257</v>
+      <c r="H24" s="9">
+        <v>43749</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5070,7 +4981,7 @@
         <v>131</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>3</v>
@@ -5078,11 +4989,11 @@
       <c r="G25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="9" t="s">
-        <v>257</v>
+      <c r="H25" s="9">
+        <v>43749</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5090,7 +5001,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>66</v>
@@ -5107,11 +5018,11 @@
       <c r="G26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="9" t="s">
-        <v>257</v>
+      <c r="H26" s="9">
+        <v>43749</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5119,7 +5030,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>28</v>
@@ -5136,11 +5047,11 @@
       <c r="G27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="9" t="s">
-        <v>257</v>
+      <c r="H27" s="9">
+        <v>43749</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5154,10 +5065,10 @@
         <v>30</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>3</v>
@@ -5165,11 +5076,11 @@
       <c r="G28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="9" t="s">
-        <v>257</v>
+      <c r="H28" s="9">
+        <v>43749</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5177,7 +5088,7 @@
         <v>31</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>67</v>
@@ -5186,7 +5097,7 @@
         <v>124</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>3</v>
@@ -5194,11 +5105,11 @@
       <c r="G29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>257</v>
+      <c r="H29" s="9">
+        <v>43749</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -5212,10 +5123,10 @@
         <v>33</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>3</v>
@@ -5223,28 +5134,28 @@
       <c r="G30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>257</v>
+      <c r="H30" s="9">
+        <v>43749</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="23" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B31" s="24">
         <v>9.1</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>3</v>
@@ -5252,28 +5163,28 @@
       <c r="G31" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>257</v>
+      <c r="H31" s="9">
+        <v>43749</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="19" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B32" s="26">
         <v>9.1999999999999993</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>3</v>
@@ -5281,11 +5192,11 @@
       <c r="G32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>257</v>
+      <c r="H32" s="9">
+        <v>43749</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5310,11 +5221,11 @@
       <c r="G33" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="9" t="s">
-        <v>257</v>
+      <c r="H33" s="9">
+        <v>43749</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5325,13 +5236,13 @@
         <v>9.4</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>3</v>
@@ -5339,11 +5250,11 @@
       <c r="G34" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H34" s="9" t="s">
-        <v>257</v>
+      <c r="H34" s="9">
+        <v>43749</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -5360,7 +5271,7 @@
         <v>136</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>3</v>
@@ -5368,11 +5279,11 @@
       <c r="G35" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="9" t="s">
-        <v>257</v>
+      <c r="H35" s="9">
+        <v>43749</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5380,16 +5291,16 @@
         <v>36</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>3</v>
@@ -5397,11 +5308,11 @@
       <c r="G36" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>257</v>
+      <c r="H36" s="9">
+        <v>43749</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5409,16 +5320,16 @@
         <v>69</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>37</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>3</v>
@@ -5426,11 +5337,11 @@
       <c r="G37" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="9" t="s">
-        <v>257</v>
+      <c r="H37" s="9">
+        <v>43749</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5438,7 +5349,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>39</v>
@@ -5455,11 +5366,11 @@
       <c r="G38" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H38" s="9" t="s">
-        <v>257</v>
+      <c r="H38" s="9">
+        <v>43749</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5476,7 +5387,7 @@
         <v>139</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>3</v>
@@ -5484,19 +5395,19 @@
       <c r="G39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="9" t="s">
-        <v>257</v>
+      <c r="H39" s="9">
+        <v>43749</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>70</v>
@@ -5513,28 +5424,28 @@
       <c r="G40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="9" t="s">
-        <v>257</v>
+      <c r="H40" s="9">
+        <v>43749</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="16" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>3</v>
@@ -5542,11 +5453,11 @@
       <c r="G41" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H41" s="9" t="s">
-        <v>257</v>
+      <c r="H41" s="9">
+        <v>43749</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5554,16 +5465,16 @@
         <v>42</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>3</v>
@@ -5571,19 +5482,19 @@
       <c r="G42" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H42" s="9" t="s">
-        <v>257</v>
+      <c r="H42" s="9">
+        <v>43749</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>44</v>
@@ -5600,28 +5511,28 @@
       <c r="G43" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H43" s="9" t="s">
-        <v>257</v>
+      <c r="H43" s="9">
+        <v>43749</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>231</v>
-      </c>
       <c r="D44" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>3</v>
@@ -5629,11 +5540,11 @@
       <c r="G44" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H44" s="9" t="s">
-        <v>257</v>
+      <c r="H44" s="9">
+        <v>43749</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5650,7 +5561,7 @@
         <v>144</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>3</v>
@@ -5658,11 +5569,11 @@
       <c r="G45" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H45" s="9" t="s">
-        <v>257</v>
+      <c r="H45" s="9">
+        <v>43749</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -5670,16 +5581,16 @@
         <v>72</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>3</v>
@@ -5687,11 +5598,11 @@
       <c r="G46" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H46" s="9" t="s">
-        <v>257</v>
+      <c r="H46" s="9">
+        <v>43749</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="10" customFormat="1" ht="23.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -5699,16 +5610,16 @@
         <v>73</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>75</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>3</v>
@@ -5716,11 +5627,11 @@
       <c r="G47" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H47" s="9" t="s">
-        <v>257</v>
+      <c r="H47" s="9">
+        <v>43749</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5728,16 +5639,16 @@
         <v>74</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>3</v>
@@ -5745,11 +5656,11 @@
       <c r="G48" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H48" s="9" t="s">
-        <v>257</v>
+      <c r="H48" s="9">
+        <v>43749</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -5766,7 +5677,7 @@
         <v>145</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>3</v>
@@ -5774,11 +5685,11 @@
       <c r="G49" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H49" s="9" t="s">
-        <v>257</v>
+      <c r="H49" s="9">
+        <v>43749</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -5795,7 +5706,7 @@
         <v>146</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>3</v>
@@ -5803,11 +5714,11 @@
       <c r="G50" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H50" s="9" t="s">
-        <v>257</v>
+      <c r="H50" s="9">
+        <v>43749</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5815,16 +5726,16 @@
         <v>80</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>147</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>3</v>
@@ -5832,11 +5743,11 @@
       <c r="G51" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H51" s="9" t="s">
-        <v>257</v>
+      <c r="H51" s="9">
+        <v>43749</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5844,7 +5755,7 @@
         <v>81</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>82</v>
@@ -5861,11 +5772,11 @@
       <c r="G52" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H52" s="9" t="s">
-        <v>257</v>
+      <c r="H52" s="9">
+        <v>43749</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5882,7 +5793,7 @@
         <v>150</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>3</v>
@@ -5890,11 +5801,11 @@
       <c r="G53" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H53" s="9" t="s">
-        <v>257</v>
+      <c r="H53" s="9">
+        <v>43749</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -5902,7 +5813,7 @@
         <v>85</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>86</v>
@@ -5911,7 +5822,7 @@
         <v>151</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>3</v>
@@ -5919,11 +5830,11 @@
       <c r="G54" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H54" s="9" t="s">
-        <v>257</v>
+      <c r="H54" s="9">
+        <v>43749</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -5940,7 +5851,7 @@
         <v>152</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>3</v>
@@ -5948,28 +5859,28 @@
       <c r="G55" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H55" s="9" t="s">
-        <v>257</v>
+      <c r="H55" s="9">
+        <v>43749</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="16" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B56" s="19">
         <v>16.100000000000001</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>269</v>
+        <v>291</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>260</v>
+        <v>292</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>3</v>
@@ -5977,11 +5888,11 @@
       <c r="G56" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H56" s="9" t="s">
-        <v>257</v>
+      <c r="H56" s="9">
+        <v>43749</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5992,7 +5903,7 @@
         <v>16.2</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>153</v>
@@ -6006,28 +5917,28 @@
       <c r="G57" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="9" t="s">
-        <v>257</v>
+      <c r="H57" s="9">
+        <v>43749</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="10" customFormat="1" ht="24.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="16" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B58" s="19">
         <v>16.3</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>3</v>
@@ -6035,16 +5946,16 @@
       <c r="G58" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H58" s="9" t="s">
-        <v>257</v>
+      <c r="H58" s="9">
+        <v>43749</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="16" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B59" s="19">
         <v>16.399999999999999</v>
@@ -6053,7 +5964,7 @@
         <v>90</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>156</v>
+        <v>289</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>111</v>
@@ -6064,16 +5975,16 @@
       <c r="G59" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H59" s="9" t="s">
-        <v>257</v>
+      <c r="H59" s="9">
+        <v>43749</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B60" s="19">
         <v>16.5</v>
@@ -6082,7 +5993,7 @@
         <v>91</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>157</v>
+        <v>290</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>155</v>
@@ -6093,11 +6004,11 @@
       <c r="G60" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H60" s="9" t="s">
-        <v>257</v>
+      <c r="H60" s="9">
+        <v>43749</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6111,10 +6022,10 @@
         <v>93</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>3</v>
@@ -6122,11 +6033,11 @@
       <c r="G61" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H61" s="9" t="s">
-        <v>257</v>
+      <c r="H61" s="9">
+        <v>43749</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6134,16 +6045,16 @@
         <v>94</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>95</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F62" s="8" t="s">
         <v>3</v>
@@ -6151,28 +6062,28 @@
       <c r="G62" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H62" s="9" t="s">
-        <v>257</v>
+      <c r="H62" s="9">
+        <v>43749</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="16" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B63" s="19">
         <v>18</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>3</v>
@@ -6180,11 +6091,11 @@
       <c r="G63" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H63" s="9" t="s">
-        <v>257</v>
+      <c r="H63" s="9">
+        <v>43749</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="10" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -6198,10 +6109,10 @@
         <v>96</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>3</v>
@@ -6209,11 +6120,11 @@
       <c r="G64" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H64" s="9" t="s">
-        <v>257</v>
+      <c r="H64" s="9">
+        <v>43749</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="10" customFormat="1" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -6227,10 +6138,10 @@
         <v>98</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>3</v>
@@ -6238,11 +6149,11 @@
       <c r="G65" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H65" s="9" t="s">
-        <v>257</v>
+      <c r="H65" s="9">
+        <v>43749</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="10" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
@@ -6256,10 +6167,10 @@
         <v>100</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>3</v>
@@ -6267,11 +6178,11 @@
       <c r="G66" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H66" s="9" t="s">
-        <v>257</v>
+      <c r="H66" s="9">
+        <v>43749</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6285,10 +6196,10 @@
         <v>102</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>3</v>
@@ -6296,16 +6207,16 @@
       <c r="G67" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H67" s="9" t="s">
-        <v>257</v>
+      <c r="H67" s="9">
+        <v>43749</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="16" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B68" s="19">
         <v>23</v>
@@ -6314,10 +6225,10 @@
         <v>104</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>3</v>
@@ -6325,11 +6236,11 @@
       <c r="G68" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H68" s="9" t="s">
-        <v>257</v>
+      <c r="H68" s="9">
+        <v>43749</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>